<commit_message>
add problem 7 description
</commit_message>
<xml_diff>
--- a/Taller4/AlgoritmosGeneticos/resultados_population.xlsx
+++ b/Taller4/AlgoritmosGeneticos/resultados_population.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,10 +447,642 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B3" t="n">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>30</v>
+      </c>
+      <c r="B4" t="n">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>40</v>
+      </c>
+      <c r="B5" t="n">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>50</v>
+      </c>
+      <c r="B6" t="n">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>60</v>
+      </c>
+      <c r="B7" t="n">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>70</v>
+      </c>
+      <c r="B8" t="n">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>80</v>
+      </c>
+      <c r="B9" t="n">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>90</v>
+      </c>
+      <c r="B10" t="n">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>100</v>
+      </c>
+      <c r="B11" t="n">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>110</v>
+      </c>
+      <c r="B12" t="n">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>120</v>
+      </c>
+      <c r="B13" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>130</v>
+      </c>
+      <c r="B14" t="n">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>140</v>
+      </c>
+      <c r="B15" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>150</v>
+      </c>
+      <c r="B16" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>160</v>
+      </c>
+      <c r="B17" t="n">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>170</v>
+      </c>
+      <c r="B18" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>180</v>
+      </c>
+      <c r="B19" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>190</v>
+      </c>
+      <c r="B20" t="n">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>200</v>
+      </c>
+      <c r="B21" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>210</v>
+      </c>
+      <c r="B22" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>220</v>
+      </c>
+      <c r="B23" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>230</v>
+      </c>
+      <c r="B24" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>240</v>
+      </c>
+      <c r="B25" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>250</v>
+      </c>
+      <c r="B26" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>260</v>
+      </c>
+      <c r="B27" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>270</v>
+      </c>
+      <c r="B28" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>280</v>
+      </c>
+      <c r="B29" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>290</v>
+      </c>
+      <c r="B30" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>300</v>
+      </c>
+      <c r="B31" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>310</v>
+      </c>
+      <c r="B32" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>320</v>
+      </c>
+      <c r="B33" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>330</v>
+      </c>
+      <c r="B34" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>340</v>
+      </c>
+      <c r="B35" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>350</v>
+      </c>
+      <c r="B36" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>360</v>
+      </c>
+      <c r="B37" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>370</v>
+      </c>
+      <c r="B38" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>380</v>
+      </c>
+      <c r="B39" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>390</v>
+      </c>
+      <c r="B40" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>400</v>
+      </c>
+      <c r="B41" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>410</v>
+      </c>
+      <c r="B42" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>420</v>
+      </c>
+      <c r="B43" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>430</v>
+      </c>
+      <c r="B44" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>440</v>
+      </c>
+      <c r="B45" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>450</v>
+      </c>
+      <c r="B46" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>460</v>
+      </c>
+      <c r="B47" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>470</v>
+      </c>
+      <c r="B48" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>480</v>
+      </c>
+      <c r="B49" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>490</v>
+      </c>
+      <c r="B50" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>500</v>
+      </c>
+      <c r="B51" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>510</v>
+      </c>
+      <c r="B52" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>520</v>
+      </c>
+      <c r="B53" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>530</v>
+      </c>
+      <c r="B54" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>540</v>
+      </c>
+      <c r="B55" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>550</v>
+      </c>
+      <c r="B56" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>560</v>
+      </c>
+      <c r="B57" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>570</v>
+      </c>
+      <c r="B58" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>580</v>
+      </c>
+      <c r="B59" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>590</v>
+      </c>
+      <c r="B60" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>600</v>
+      </c>
+      <c r="B61" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>610</v>
+      </c>
+      <c r="B62" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>620</v>
+      </c>
+      <c r="B63" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>630</v>
+      </c>
+      <c r="B64" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>640</v>
+      </c>
+      <c r="B65" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>650</v>
+      </c>
+      <c r="B66" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>660</v>
+      </c>
+      <c r="B67" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>670</v>
+      </c>
+      <c r="B68" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
         <v>680</v>
       </c>
-      <c r="B2" t="n">
-        <v>18</v>
+      <c r="B69" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>690</v>
+      </c>
+      <c r="B70" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>700</v>
+      </c>
+      <c r="B71" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>710</v>
+      </c>
+      <c r="B72" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>720</v>
+      </c>
+      <c r="B73" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>730</v>
+      </c>
+      <c r="B74" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>740</v>
+      </c>
+      <c r="B75" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>750</v>
+      </c>
+      <c r="B76" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>760</v>
+      </c>
+      <c r="B77" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>770</v>
+      </c>
+      <c r="B78" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>780</v>
+      </c>
+      <c r="B79" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>790</v>
+      </c>
+      <c r="B80" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>800</v>
+      </c>
+      <c r="B81" t="n">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>